<commit_message>
Updated ActivityDiagram.gliffy and ActivityDiagram.png
</commit_message>
<xml_diff>
--- a/Documentation/SQA Checklist.xlsx
+++ b/Documentation/SQA Checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
   <si>
     <t>Task ID</t>
   </si>
@@ -160,6 +160,27 @@
   </si>
   <si>
     <t>Quality Assurance Testing Timeline for &lt;Release x.x&gt;</t>
+  </si>
+  <si>
+    <t>Databse</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>BI tool</t>
+  </si>
+  <si>
+    <t>Log In system</t>
+  </si>
+  <si>
+    <t>Request supplies</t>
+  </si>
+  <si>
+    <t>Forms</t>
+  </si>
+  <si>
+    <t>List of supplies</t>
   </si>
 </sst>
 </file>
@@ -222,7 +243,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -245,26 +266,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -293,6 +311,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,525 +618,547 @@
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="58.28515625" customWidth="1"/>
     <col min="4" max="9" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="K3" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="K4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8" t="s">
+      <c r="D5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="K5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="5">
         <v>40435</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="5">
         <v>40436</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="6">
         <v>0.8</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8" t="s">
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="K6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="11" t="s">
+      <c r="D7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="K7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8">
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4">
         <v>4</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8">
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4">
         <v>5</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="K9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8">
+      <c r="D10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4">
         <v>5</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+    <row r="11" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="15" t="s">
+      <c r="D11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8">
+      <c r="D12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
         <v>7</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8" t="s">
+      <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="11" t="s">
+      <c r="D14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+    <row r="15" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8">
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
         <v>11</v>
       </c>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8">
+      <c r="D16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
         <v>12</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="4">
         <v>14</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8">
+      <c r="D17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
         <v>13</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8">
+      <c r="D18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4">
         <v>14</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8">
+      <c r="D19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
         <v>15</v>
       </c>
-      <c r="I19" s="8"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8">
+      <c r="D20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4">
         <v>16</v>
       </c>
-      <c r="I20" s="8"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8">
+      <c r="D21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4">
         <v>17</v>
       </c>
-      <c r="I21" s="8"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8">
+      <c r="D22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4">
         <v>18</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="A23" s="11">
         <v>20</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="17" t="s">
+      <c r="D23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="I23" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="A24" s="11">
         <v>21</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="16" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="17" t="s">
+      <c r="D24" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="15" t="s">
+      <c r="I24" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="A25" s="11">
         <v>22</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="17" t="s">
+      <c r="D25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="A26" s="11">
         <v>23</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15">
+      <c r="D26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11">
         <v>22</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="11" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated but not yet final SQA Checklist
</commit_message>
<xml_diff>
--- a/Documentation/SQA Checklist.xlsx
+++ b/Documentation/SQA Checklist.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Task ID</t>
   </si>
@@ -27,69 +28,6 @@
     <t>Task Name</t>
   </si>
   <si>
-    <t>&lt;Release x.x&gt; Code Freeze</t>
-  </si>
-  <si>
-    <t>(Unit, Functional) Test Completion</t>
-  </si>
-  <si>
-    <t>Unit testing by developer</t>
-  </si>
-  <si>
-    <t>Rework and fix any issues found by developers</t>
-  </si>
-  <si>
-    <t>Unit test reverification by developers</t>
-  </si>
-  <si>
-    <t>Engineering Test Completetion sign-off</t>
-  </si>
-  <si>
-    <t>Deploy Code to QA test server</t>
-  </si>
-  <si>
-    <t>Create Change Request Form for Release and send to the Change Advisor board for reaview and approval</t>
-  </si>
-  <si>
-    <t>Official start of QA Testing &lt;Release x.x&gt;</t>
-  </si>
-  <si>
-    <t>Create Fix testing scripts &lt;Release x.x&gt;</t>
-  </si>
-  <si>
-    <t>Start Fix testing &lt;Release x.x&gt;</t>
-  </si>
-  <si>
-    <t>Rework and fixes any issues found by QA Tester as documented in defect tracking application</t>
-  </si>
-  <si>
-    <t>Reverification of fixed issues by QA Tester</t>
-  </si>
-  <si>
-    <t>Send Fix testing Status sign-off</t>
-  </si>
-  <si>
-    <t>Regression testing &lt;Release x.x&gt;</t>
-  </si>
-  <si>
-    <t>Restart and complete regression testing to QA tester</t>
-  </si>
-  <si>
-    <t>Send Regression testing Status sign-off</t>
-  </si>
-  <si>
-    <t>Release Communication to Application clients</t>
-  </si>
-  <si>
-    <t>Complete and send Help/User Guide Documents update sign-off</t>
-  </si>
-  <si>
-    <t>Deploy &lt;Release x.x&gt; Code and User Guide to PRODUCTION</t>
-  </si>
-  <si>
-    <t>Post Production Verification of &lt;release x.x&gt;</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -181,6 +119,108 @@
   </si>
   <si>
     <t>List of supplies</t>
+  </si>
+  <si>
+    <t>Project charter approved</t>
+  </si>
+  <si>
+    <t>Project plan completed</t>
+  </si>
+  <si>
+    <t>Project plan approved</t>
+  </si>
+  <si>
+    <t>Project team assembled</t>
+  </si>
+  <si>
+    <t>Project execution initiated</t>
+  </si>
+  <si>
+    <t>Project execution completed</t>
+  </si>
+  <si>
+    <t>Customer acceptance</t>
+  </si>
+  <si>
+    <t>Project closed out</t>
+  </si>
+  <si>
+    <t>Evaluate current process of client</t>
+  </si>
+  <si>
+    <t>Propose project</t>
+  </si>
+  <si>
+    <t>Identify system process</t>
+  </si>
+  <si>
+    <t>Create Project Management Plan</t>
+  </si>
+  <si>
+    <t>Create WBS</t>
+  </si>
+  <si>
+    <t>Gantt Chart</t>
+  </si>
+  <si>
+    <t>Event Table</t>
+  </si>
+  <si>
+    <t>Use Case Diagram</t>
+  </si>
+  <si>
+    <t>Activity Diagram</t>
+  </si>
+  <si>
+    <t>Context Flow Diagram</t>
+  </si>
+  <si>
+    <t>Data Flow Diagram</t>
+  </si>
+  <si>
+    <t>Entity Relationship Diagram</t>
+  </si>
+  <si>
+    <t>Identify possible solutions</t>
+  </si>
+  <si>
+    <t>Business Intelligence Tool</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Login/Register Interface</t>
+  </si>
+  <si>
+    <t>Advisory form</t>
+  </si>
+  <si>
+    <t>LGU basic information form</t>
+  </si>
+  <si>
+    <t>Request supply form</t>
+  </si>
+  <si>
+    <t>List of accounts grid view</t>
+  </si>
+  <si>
+    <t>List of requests grid view</t>
+  </si>
+  <si>
+    <t>Historical data form</t>
+  </si>
+  <si>
+    <t>Add and update data</t>
+  </si>
+  <si>
+    <t>Working Business Intelligence tool</t>
+  </si>
+  <si>
+    <t>Working database</t>
+  </si>
+  <si>
+    <t>Complete proof of concept for system</t>
   </si>
 </sst>
 </file>
@@ -189,14 +229,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -234,6 +266,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -243,7 +281,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -275,11 +313,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -296,36 +356,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,30 +690,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="A1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="A2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -656,25 +724,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -682,8 +750,8 @@
         <v>1</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
+      <c r="C4" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -691,10 +759,10 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -702,21 +770,21 @@
         <v>2</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
+      <c r="C5" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -724,11 +792,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
+      <c r="C6" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E6" s="5">
         <v>40435</v>
@@ -741,10 +809,10 @@
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -752,23 +820,23 @@
         <v>4</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
+      <c r="C7" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="7" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -776,11 +844,11 @@
         <v>5</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
+      <c r="C8" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -789,10 +857,10 @@
         <v>4</v>
       </c>
       <c r="I8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
         <v>31</v>
-      </c>
-      <c r="K8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -800,11 +868,11 @@
         <v>6</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
+      <c r="C9" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -813,10 +881,10 @@
         <v>5</v>
       </c>
       <c r="I9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" t="s">
         <v>32</v>
-      </c>
-      <c r="K9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -824,11 +892,11 @@
         <v>7</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="8" t="s">
-        <v>8</v>
+      <c r="C10" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -837,7 +905,7 @@
         <v>5</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -845,18 +913,18 @@
         <v>8</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="9" t="s">
-        <v>9</v>
+      <c r="C11" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="11" t="s">
-        <v>37</v>
+      <c r="I11" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -864,11 +932,11 @@
         <v>9</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="8" t="s">
-        <v>10</v>
+      <c r="C12" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -877,7 +945,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -885,18 +953,18 @@
         <v>10</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>11</v>
+      <c r="C13" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -904,20 +972,20 @@
         <v>11</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
-        <v>12</v>
+      <c r="C14" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="7" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -925,11 +993,11 @@
         <v>12</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="10" t="s">
-        <v>13</v>
+      <c r="C15" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -944,11 +1012,11 @@
         <v>13</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="4" t="s">
-        <v>14</v>
+      <c r="C16" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -963,11 +1031,11 @@
         <v>14</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="4" t="s">
-        <v>15</v>
+      <c r="C17" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -976,7 +1044,7 @@
         <v>13</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -984,11 +1052,11 @@
         <v>15</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
-        <v>16</v>
+      <c r="C18" s="16" t="s">
+        <v>55</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -997,170 +1065,220 @@
         <v>14</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>16</v>
-      </c>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="4">
-        <v>15</v>
-      </c>
+      <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
-        <v>14</v>
+      <c r="C20" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="4" t="s">
-        <v>17</v>
+      <c r="C21" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
-        <v>18</v>
+      <c r="C22" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4">
+        <v>17</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>19</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4">
         <v>18</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="I23" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
         <v>20</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="B24" s="8"/>
+      <c r="C24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
         <v>21</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="B25" s="8"/>
+      <c r="C25" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
         <v>22</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="B26" s="8"/>
+      <c r="C26" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
         <v>23</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="12" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8">
         <v>22</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11">
-        <v>22</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="I27" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1170,4 +1288,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>